<commit_message>
updating some incorrect analyses
</commit_message>
<xml_diff>
--- a/item_Analysis.Tables.xlsx
+++ b/item_Analysis.Tables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abbievannuland/Documents/GitHub/SPP-Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebuchanan\OneDrive - Harrisburg University\RESEARCH\2 projects\SPP-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_0C8E74689ACAF3097C5CB247FA92566A3845E052" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{BFE2CAF2-6C20-4205-AE30-A8A1E49BFA65}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="460" windowWidth="19840" windowHeight="16100" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="3645" yWindow="465" windowWidth="19845" windowHeight="16095" tabRatio="500" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SOA200, other, ldt" sheetId="2" r:id="rId1"/>
@@ -21,8 +22,13 @@
     <sheet name="SOA1200, other, naming" sheetId="8" r:id="rId7"/>
     <sheet name="SOA1200, first, naming" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2502" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2503" uniqueCount="68">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -233,11 +239,14 @@
   <si>
     <t>model.3a.d</t>
   </si>
+  <si>
+    <t>Don't forget you updated this</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
@@ -668,49 +677,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="AD27" sqref="AD27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="4" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="4"/>
+    <col min="29" max="29" width="4.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
@@ -799,7 +808,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -864,7 +873,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -929,7 +938,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -994,7 +1003,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -1053,7 +1062,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1106,7 +1115,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1141,7 +1150,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1173,7 +1182,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -1227,7 +1236,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -1277,7 +1286,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -1327,7 +1336,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -1359,7 +1368,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -1391,7 +1400,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
@@ -1420,7 +1429,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -1450,7 +1459,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -1479,7 +1488,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
@@ -1505,7 +1514,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
@@ -1549,7 +1558,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -1569,7 +1578,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -1586,7 +1595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>48</v>
       </c>
@@ -1606,7 +1615,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
@@ -1626,7 +1635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
@@ -1643,7 +1652,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
@@ -1661,7 +1670,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
@@ -1678,7 +1687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
@@ -1692,7 +1701,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -1728,7 +1737,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
@@ -1739,7 +1748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>59</v>
       </c>
@@ -1747,7 +1756,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
@@ -1758,7 +1767,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
@@ -1769,7 +1778,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -1777,7 +1786,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
@@ -1786,7 +1795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
@@ -1794,7 +1803,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
@@ -1805,49 +1814,49 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="4" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="4"/>
+    <col min="29" max="29" width="4.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
@@ -1936,7 +1945,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -1998,7 +2007,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -2058,7 +2067,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -2117,7 +2126,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -2179,7 +2188,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -2233,7 +2242,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
@@ -2268,7 +2277,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
@@ -2300,7 +2309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -2354,7 +2363,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -2404,7 +2413,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -2454,7 +2463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>43</v>
       </c>
@@ -2486,7 +2495,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>44</v>
       </c>
@@ -2518,7 +2527,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>27</v>
       </c>
@@ -2547,7 +2556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>45</v>
       </c>
@@ -2577,7 +2586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>46</v>
       </c>
@@ -2606,7 +2615,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>47</v>
       </c>
@@ -2632,7 +2641,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
@@ -2674,7 +2683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>49</v>
       </c>
@@ -2694,7 +2703,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>51</v>
       </c>
@@ -2711,7 +2720,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>48</v>
       </c>
@@ -2731,7 +2740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>53</v>
       </c>
@@ -2751,7 +2760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>52</v>
       </c>
@@ -2768,7 +2777,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>54</v>
       </c>
@@ -2786,7 +2795,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>55</v>
       </c>
@@ -2803,7 +2812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>56</v>
       </c>
@@ -2817,7 +2826,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -2850,7 +2859,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>58</v>
       </c>
@@ -2861,7 +2870,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>59</v>
       </c>
@@ -2869,7 +2878,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>60</v>
       </c>
@@ -2880,7 +2889,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>61</v>
       </c>
@@ -2891,7 +2900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>62</v>
       </c>
@@ -2899,7 +2908,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>63</v>
       </c>
@@ -2908,7 +2917,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>64</v>
       </c>
@@ -2916,7 +2925,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>65</v>
       </c>
@@ -2928,49 +2937,49 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView zoomScale="157" zoomScaleNormal="251" zoomScalePageLayoutView="251" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="4" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="4"/>
+    <col min="29" max="29" width="4.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
@@ -3059,7 +3068,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -3118,7 +3127,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -3175,7 +3184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -3231,7 +3240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -3284,7 +3293,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -3338,7 +3347,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>21</v>
       </c>
@@ -3373,7 +3382,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>22</v>
       </c>
@@ -3405,7 +3414,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -3456,7 +3465,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -3506,7 +3515,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -3553,7 +3562,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>43</v>
       </c>
@@ -3585,7 +3594,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>44</v>
       </c>
@@ -3617,7 +3626,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
@@ -3646,7 +3655,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>45</v>
       </c>
@@ -3676,7 +3685,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>46</v>
       </c>
@@ -3705,7 +3714,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>47</v>
       </c>
@@ -3731,7 +3740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
@@ -3767,7 +3776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>49</v>
       </c>
@@ -3787,7 +3796,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>51</v>
       </c>
@@ -3804,7 +3813,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>48</v>
       </c>
@@ -3824,7 +3833,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>53</v>
       </c>
@@ -3844,7 +3853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>52</v>
       </c>
@@ -3861,7 +3870,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>54</v>
       </c>
@@ -3879,7 +3888,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>55</v>
       </c>
@@ -3896,7 +3905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>56</v>
       </c>
@@ -3910,7 +3919,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -3937,7 +3946,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>58</v>
       </c>
@@ -3948,7 +3957,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>59</v>
       </c>
@@ -3956,7 +3965,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>60</v>
       </c>
@@ -3967,7 +3976,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>61</v>
       </c>
@@ -3978,7 +3987,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>62</v>
       </c>
@@ -3986,7 +3995,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>63</v>
       </c>
@@ -3995,7 +4004,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>64</v>
       </c>
@@ -4003,7 +4012,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>65</v>
       </c>
@@ -4015,49 +4024,49 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="4" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="4"/>
+    <col min="29" max="29" width="4.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
@@ -4146,7 +4155,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -4214,7 +4223,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -4280,7 +4289,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -4345,7 +4354,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -4404,7 +4413,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -4464,7 +4473,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -4499,7 +4508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -4531,7 +4540,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -4591,7 +4600,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -4647,7 +4656,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -4703,7 +4712,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -4735,7 +4744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -4767,7 +4776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
@@ -4796,7 +4805,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -4826,7 +4835,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -4855,7 +4864,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
@@ -4881,7 +4890,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
@@ -4929,7 +4938,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -4949,7 +4958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -4966,7 +4975,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>48</v>
       </c>
@@ -4986,7 +4995,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
@@ -5006,7 +5015,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
@@ -5023,7 +5032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
@@ -5041,7 +5050,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
@@ -5058,7 +5067,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
@@ -5072,7 +5081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -5117,7 +5126,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
@@ -5128,7 +5137,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>59</v>
       </c>
@@ -5136,7 +5145,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
@@ -5147,7 +5156,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
@@ -5158,7 +5167,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -5166,7 +5175,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
@@ -5175,7 +5184,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
@@ -5183,7 +5192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
@@ -5194,49 +5203,49 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="4" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="4"/>
+    <col min="29" max="29" width="4.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
@@ -5325,7 +5334,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -5387,7 +5396,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -5452,7 +5461,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -5514,7 +5523,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -5570,7 +5579,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -5623,7 +5632,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -5658,7 +5667,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -5690,7 +5699,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -5743,7 +5752,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -5793,7 +5802,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -5840,7 +5849,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -5872,7 +5881,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -5904,7 +5913,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
@@ -5933,7 +5942,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -5963,7 +5972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
@@ -5992,7 +6001,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
@@ -6018,7 +6027,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
@@ -6039,7 +6048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -6059,7 +6068,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -6076,7 +6085,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>48</v>
       </c>
@@ -6096,7 +6105,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
@@ -6116,7 +6125,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
@@ -6133,7 +6142,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
@@ -6151,7 +6160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
@@ -6168,7 +6177,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
@@ -6182,7 +6191,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -6211,7 +6220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
@@ -6222,7 +6231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>59</v>
       </c>
@@ -6230,7 +6239,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>60</v>
       </c>
@@ -6241,7 +6250,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
@@ -6252,7 +6261,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -6260,7 +6269,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
@@ -6269,7 +6278,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
@@ -6277,7 +6286,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
@@ -6288,49 +6297,49 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="4" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="4"/>
+    <col min="29" max="29" width="4.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
@@ -6419,7 +6428,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -6481,7 +6490,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -6546,7 +6555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -6614,7 +6623,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -6673,7 +6682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -6738,7 +6747,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -6792,7 +6801,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -6844,7 +6853,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -6896,7 +6905,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -6948,7 +6957,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -7010,7 +7019,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>66</v>
       </c>
@@ -7045,7 +7054,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>43</v>
       </c>
@@ -7097,7 +7106,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>44</v>
       </c>
@@ -7149,7 +7158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
@@ -7199,7 +7208,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>45</v>
       </c>
@@ -7249,7 +7258,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
@@ -7299,7 +7308,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>47</v>
       </c>
@@ -7347,7 +7356,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>50</v>
       </c>
@@ -7391,7 +7400,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>49</v>
       </c>
@@ -7435,7 +7444,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>51</v>
       </c>
@@ -7485,7 +7494,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>48</v>
       </c>
@@ -7529,7 +7538,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>53</v>
       </c>
@@ -7573,7 +7582,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>52</v>
       </c>
@@ -7615,7 +7624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>54</v>
       </c>
@@ -7657,7 +7666,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>55</v>
       </c>
@@ -7699,7 +7708,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>56</v>
       </c>
@@ -7739,7 +7748,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>57</v>
       </c>
@@ -7777,7 +7786,7 @@
       <c r="AC28" s="2"/>
       <c r="AD28" s="2"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>58</v>
       </c>
@@ -7815,7 +7824,7 @@
       <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>59</v>
       </c>
@@ -7847,7 +7856,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>60</v>
       </c>
@@ -7885,7 +7894,7 @@
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>61</v>
       </c>
@@ -7923,7 +7932,7 @@
       <c r="AC32" s="2"/>
       <c r="AD32" s="2"/>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>62</v>
       </c>
@@ -7959,7 +7968,7 @@
       <c r="AC33" s="2"/>
       <c r="AD33" s="2"/>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>63</v>
       </c>
@@ -7995,7 +8004,7 @@
       <c r="AC34" s="2"/>
       <c r="AD34" s="2"/>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>64</v>
       </c>
@@ -8031,7 +8040,7 @@
       <c r="AC35" s="2"/>
       <c r="AD35" s="2"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>65</v>
       </c>
@@ -8071,7 +8080,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8079,42 +8088,42 @@
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.375" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.375" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.125" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.875" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="5" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.625" style="4" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="10.83203125" style="4"/>
+    <col min="29" max="29" width="4.125" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>23</v>
       </c>
@@ -8203,7 +8212,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -8262,7 +8271,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -8322,7 +8331,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -8381,7 +8390,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -8437,7 +8446,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -8491,7 +8500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -8526,7 +8535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -8558,7 +8567,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>41</v>
       </c>
@@ -8609,7 +8618,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -8659,7 +8668,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
@@ -8706,7 +8715,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -8738,7 +8747,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>44</v>
       </c>
@@ -8770,7 +8779,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -8799,7 +8808,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>45</v>
       </c>
@@ -8829,7 +8838,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>46</v>
       </c>
@@ -8858,7 +8867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>47</v>
       </c>
@@ -8884,7 +8893,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
@@ -8923,7 +8932,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>49</v>
       </c>
@@ -8949,7 +8958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>51</v>
       </c>
@@ -8966,7 +8975,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
@@ -8986,7 +8995,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>53</v>
       </c>
@@ -9006,7 +9015,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>52</v>
       </c>
@@ -9023,7 +9032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>54</v>
       </c>
@@ -9041,7 +9050,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>55</v>
       </c>
@@ -9058,7 +9067,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>56</v>
       </c>
@@ -9072,7 +9081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -9102,7 +9111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>58</v>
       </c>
@@ -9113,7 +9122,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>59</v>
       </c>
@@ -9121,7 +9130,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>60</v>
       </c>
@@ -9132,7 +9141,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>61</v>
       </c>
@@ -9143,7 +9152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>62</v>
       </c>
@@ -9151,7 +9160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>63</v>
       </c>
@@ -9160,7 +9169,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>64</v>
       </c>
@@ -9168,7 +9177,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>65</v>
       </c>
@@ -9179,20 +9188,20 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:AD37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
@@ -9281,7 +9290,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -9343,7 +9352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -9377,7 +9386,7 @@
       <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -9414,7 +9423,7 @@
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -9444,12 +9453,12 @@
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
     </row>
-    <row r="6" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -9502,7 +9511,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
@@ -9534,7 +9543,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>41</v>
       </c>
@@ -9566,7 +9575,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>42</v>
       </c>
@@ -9598,7 +9607,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -9627,7 +9636,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -9677,7 +9686,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>44</v>
       </c>
@@ -9727,7 +9736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
@@ -9774,7 +9783,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>45</v>
       </c>
@@ -9803,7 +9812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>46</v>
       </c>
@@ -9832,7 +9841,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>47</v>
       </c>
@@ -9861,22 +9870,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
@@ -9910,47 +9919,47 @@
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
     </row>
-    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>60</v>
       </c>
@@ -9981,29 +9990,34 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="33" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>